<commit_message>
Regen: Remove stray note about CODEX analyte
</commit_message>
<xml_diff>
--- a/docs/lcms/lcms-metadata.xlsx
+++ b/docs/lcms/lcms-metadata.xlsx
@@ -12,10 +12,16 @@
     <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
     <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
     <sheet name="analyte_class list" sheetId="5" r:id="rId5"/>
-    <sheet name="lc_length_unit list" sheetId="6" r:id="rId6"/>
-    <sheet name="lc_temp_unit list" sheetId="7" r:id="rId7"/>
-    <sheet name="lc_id_unit list" sheetId="8" r:id="rId8"/>
-    <sheet name="lc_flow_rate_unit list" sheetId="9" r:id="rId9"/>
+    <sheet name="ms_source list" sheetId="6" r:id="rId6"/>
+    <sheet name="ion_mobility list" sheetId="7" r:id="rId7"/>
+    <sheet name="lc_length_unit list" sheetId="8" r:id="rId8"/>
+    <sheet name="lc_temp_unit list" sheetId="9" r:id="rId9"/>
+    <sheet name="lc_id_unit list" sheetId="10" r:id="rId10"/>
+    <sheet name="lc_flow_rate_unit list" sheetId="11" r:id="rId11"/>
+    <sheet name="spatial_type list" sheetId="12" r:id="rId12"/>
+    <sheet name="spatial_sampling_type list" sheetId="13" r:id="rId13"/>
+    <sheet name="resolution_x_unit list" sheetId="14" r:id="rId14"/>
+    <sheet name="resolution_y_unit list" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -205,7 +211,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specifies whether or not a specific molecule(s) is/are targeted for detection/measurement by the assay. The CODEX analyte is protein.</t>
+          <t>Specifies whether or not a specific molecule(s) is/are targeted for detection/measurement by the assay.</t>
         </r>
       </text>
     </comment>
@@ -244,7 +250,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The ion source type used for surface sampling (MALDI, MALDI-2, DESI, or SIMS) or LC-MS/MS data acquisition (nESI)</t>
+          <t>The ion source type used for surface sampling.</t>
         </r>
       </text>
     </comment>
@@ -296,11 +302,50 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>This is the MS1 resolving power. This is a unitless value often calculated as m/∆m where ∆m is the FWHM for a given peak with a certain m/z (m).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The peak (m/z) used to calculate the resolving power.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not ion mobility spectrometry was performed and which technology was used. Technologies for measuring ion mobility: Traveling Wave Ion Mobility Spectrometry (TWIMS), Trapped Ion Mobility Spectrometry (TIMS), High Field Asymmetric waveform ion Mobility Spectrometry (FAIMS), Drift Tube Ion Mobility Spectrometry (DTIMS, Structures for Lossless Ion Manipulations (SLIM).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Mode of data collection in tandem MS assays. Either DDA (Data-dependent acquisition) or DIA (Data-indemendent acquisition.</t>
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -313,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -326,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -339,7 +384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="AB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -352,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -365,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -378,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -391,7 +436,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -404,7 +449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +462,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -430,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -443,7 +488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -456,7 +501,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +514,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -482,7 +527,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -495,7 +540,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -508,7 +553,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -521,7 +566,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -534,7 +579,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AQ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +592,98 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
+    <comment ref="AR1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not the analysis was performed in a spatialy targeted manner and the technique used for spatial sampling. For example, Laser-capture microdissection (LCM), Liquid Extraction Surface Analysis (LESA), Nanodroplet Processing in One pot for Trace Samples (nanoPOTS).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AS1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies whether or not the analysis was performed in a spatially targeted manner. Spatial profiling experiments target specific tissue foci but do not necessarily generate images. Spatial imaging expriments collect data from a regular array (pixels) that can be visualized as heat maps of ion intensity at each location (molecular images). Leave blank if data are derived from bulk analysis.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AT1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specifies the cell-type or functional tissue unit (FTU) that is targeted in the spatial profiling experiment. Leave blank if data are generated in imaging mode without a specific target structure.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AU1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The width of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AV1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of measurement of the width of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AW1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The height of a pixel</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AX1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>The unit of measurement of the height of a pixel.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AY1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -560,7 +696,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0">
+    <comment ref="AZ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0">
+    <comment ref="BA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -586,7 +722,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AR1" authorId="0">
+    <comment ref="BB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -599,7 +735,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AS1" authorId="0">
+    <comment ref="BC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -617,12 +753,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
     <t>description</t>
@@ -661,13 +797,22 @@
     <t>assay_type</t>
   </si>
   <si>
-    <t>LC-MS (metabolomics)</t>
-  </si>
-  <si>
-    <t>LC-MS/MS (label-free proteomics)</t>
-  </si>
-  <si>
-    <t>MS (shotgun lipidomics)</t>
+    <t>LC-MS</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>LC-MS Bottom-Up</t>
+  </si>
+  <si>
+    <t>MS Bottom-Up</t>
+  </si>
+  <si>
+    <t>LC-MS Top-Down</t>
+  </si>
+  <si>
+    <t>MS Top-Down</t>
   </si>
   <si>
     <t>analyte_class</t>
@@ -682,6 +827,15 @@
     <t>lipids</t>
   </si>
   <si>
+    <t>peptides</t>
+  </si>
+  <si>
+    <t>phosphopeptides</t>
+  </si>
+  <si>
+    <t>glycans</t>
+  </si>
+  <si>
     <t>is_targeted</t>
   </si>
   <si>
@@ -694,6 +848,9 @@
     <t>ms_source</t>
   </si>
   <si>
+    <t>ESI</t>
+  </si>
+  <si>
     <t>polarity</t>
   </si>
   <si>
@@ -703,6 +860,30 @@
     <t>mz_range_high_value</t>
   </si>
   <si>
+    <t>mass_resolving_power</t>
+  </si>
+  <si>
+    <t>mz_resolving_power</t>
+  </si>
+  <si>
+    <t>ion_mobility</t>
+  </si>
+  <si>
+    <t>TIMS</t>
+  </si>
+  <si>
+    <t>TWIMS</t>
+  </si>
+  <si>
+    <t>FAIMS</t>
+  </si>
+  <si>
+    <t>DTIMS</t>
+  </si>
+  <si>
+    <t>SLIMS</t>
+  </si>
+  <si>
     <t>data_collection_mode</t>
   </si>
   <si>
@@ -779,6 +960,48 @@
   </si>
   <si>
     <t>lc_mobile_phase_b</t>
+  </si>
+  <si>
+    <t>spatial_type</t>
+  </si>
+  <si>
+    <t>LCM</t>
+  </si>
+  <si>
+    <t>LESA</t>
+  </si>
+  <si>
+    <t>nanoPOTS</t>
+  </si>
+  <si>
+    <t>microLESA</t>
+  </si>
+  <si>
+    <t>spatial_sampling_type</t>
+  </si>
+  <si>
+    <t>profiling</t>
+  </si>
+  <si>
+    <t>imaging</t>
+  </si>
+  <si>
+    <t>spatial_target</t>
+  </si>
+  <si>
+    <t>resolution_x_value</t>
+  </si>
+  <si>
+    <t>resolution_x_unit</t>
+  </si>
+  <si>
+    <t>nm</t>
+  </si>
+  <si>
+    <t>resolution_y_value</t>
+  </si>
+  <si>
+    <t>resolution_y_unit</t>
   </si>
   <si>
     <t>processing_search</t>
@@ -1142,7 +1365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS1"/>
+  <dimension ref="A1:BC1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1151,7 +1374,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:55">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1189,121 +1412,154 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+  <dataValidations count="25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 2." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: mass_spectrometry." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: LC-MS (metabolomics) / LC-MS/MS (label-free proteomics) / MS (shotgun lipidomics)." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$3</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: protein / metabolites / lipids." sqref="M2:M1048576">
-      <formula1>'analyte_class list'!$A$1:$A$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from analyte_class list." sqref="M2:M1048576">
+      <formula1>'analyte_class list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="N2:N1048576">
       <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ESI." sqref="Q2:Q1048576">
+      <formula1>'ms_source list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="S2:S1048576">
       <formula1>-1e+307</formula1>
@@ -1313,37 +1569,221 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AD2:AD1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="U2:U1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um / mm / cm." sqref="AE2:AE1048576">
-      <formula1>'lc_length_unit list'!$A$1:$A$3</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AF2:AF1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="V2:V1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: C." sqref="AG2:AG1048576">
-      <formula1>'lc_temp_unit list'!$A$1:$A$1</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AH2:AH1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: TIMS / TWIMS / FAIMS / DTIMS / SLIMS." sqref="W2:W1048576">
+      <formula1>'ion_mobility list'!$A$1:$A$5</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AG2:AG1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um / mm / cm." sqref="AI2:AI1048576">
-      <formula1>'lc_id_unit list'!$A$1:$A$3</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AJ2:AJ1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um / mm / cm." sqref="AH2:AH1048576">
+      <formula1>'lc_length_unit list'!$A$1:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AI2:AI1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nL/min / mL/min." sqref="AK2:AK1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: C." sqref="AJ2:AJ1048576">
+      <formula1>'lc_temp_unit list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AK2:AK1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: um / mm / cm." sqref="AL2:AL1048576">
+      <formula1>'lc_id_unit list'!$A$1:$A$3</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AM2:AM1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nL/min / mL/min." sqref="AN2:AN1048576">
       <formula1>'lc_flow_rate_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: LCM / LESA / nanoPOTS / microLESA." sqref="AR2:AR1048576">
+      <formula1>'spatial_type list'!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: profiling / imaging." sqref="AS2:AS1048576">
+      <formula1>'spatial_sampling_type list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AU2:AU1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="AV2:AV1048576">
+      <formula1>'resolution_x_unit list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AW2:AW1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: nm / um." sqref="AX2:AX1048576">
+      <formula1>'resolution_y_unit list'!$A$1:$A$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1385,7 +1825,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1406,6 +1846,21 @@
         <v>16</v>
       </c>
     </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1413,7 +1868,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1421,17 +1876,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1440,34 +1910,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1477,7 +1919,45 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1495,17 +1975,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1515,7 +1995,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1523,12 +2003,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>